<commit_message>
data provider with multiple scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateAirlineData.xlsx
+++ b/src/test/resources/testdata/CreateAirlineData.xlsx
@@ -506,7 +506,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>